<commit_message>
añadida mas info sobre la configuracion de la maq.
</commit_message>
<xml_diff>
--- a/Lista de tareas.xlsx
+++ b/Lista de tareas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Plasmar ese analisis en la documentación</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>actualizar el readme en github para que diga la version de tkinter que tiene que estar instalada para poder correr el programa interfaz</t>
+  </si>
+  <si>
+    <t>que la interfaz muestre todos los datos contenidos en el archivo de configuracion</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>el programa muestra tooltips sobre cada boton con los shortcuts de teclado</t>
+  </si>
+  <si>
+    <t>añadir generar cadena aleatoria como boton</t>
   </si>
 </sst>
 </file>
@@ -662,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +729,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.002479166666</v>
+        <v>44519.809722685182</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -777,7 +789,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.002479166666</v>
+        <v>44519.809722685182</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -818,7 +830,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.002479166666</v>
+        <v>44519.809722685182</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -851,7 +863,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.002479166666</v>
+        <v>44519.809722685182</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -866,7 +878,7 @@
       </c>
       <c r="D10" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.002479166666</v>
+        <v>44519.809722685182</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -884,7 +896,7 @@
       </c>
       <c r="D11" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.002479166666</v>
+        <v>44519.809722685182</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -898,8 +910,13 @@
       <c r="C12" s="3">
         <v>44517.202512268515</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="3">
+        <f ca="1">NOW()</f>
+        <v>44519.809722685182</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
@@ -907,7 +924,9 @@
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C13" s="3">
         <v>44517.88040011574</v>
       </c>
@@ -961,19 +980,27 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3">
+        <v>44519.807343749999</v>
+      </c>
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3">
+        <v>44519.807343749999</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>

</xml_diff>

<commit_message>
añadidos cambios "finales" y guia de usuario
</commit_message>
<xml_diff>
--- a/Lista de tareas.xlsx
+++ b/Lista de tareas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Plasmar ese analisis en la documentación</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>añadir generar cadena aleatoria como boton</t>
+  </si>
+  <si>
+    <t>Hecho en interfaz</t>
+  </si>
+  <si>
+    <t>hecho en readme</t>
+  </si>
+  <si>
+    <t>Hecho todo menos el boton de generar cadena random</t>
   </si>
 </sst>
 </file>
@@ -178,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -190,6 +199,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -674,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +741,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.809722685182</v>
+        <v>44519.838576620372</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -789,7 +801,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.809722685182</v>
+        <v>44519.838576620372</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
@@ -830,7 +842,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.809722685182</v>
+        <v>44519.838576620372</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -863,7 +875,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.809722685182</v>
+        <v>44519.838576620372</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
@@ -878,7 +890,7 @@
       </c>
       <c r="D10" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.809722685182</v>
+        <v>44519.838576620372</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -896,7 +908,7 @@
       </c>
       <c r="D11" s="3">
         <f ca="1">NOW()</f>
-        <v>44519.809722685182</v>
+        <v>44519.838576620372</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -910,17 +922,11 @@
       <c r="C12" s="3">
         <v>44517.202512268515</v>
       </c>
-      <c r="D12" s="3">
-        <f ca="1">NOW()</f>
-        <v>44519.809722685182</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="D12" s="5"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -930,21 +936,32 @@
       <c r="C13" s="3">
         <v>44517.88040011574</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="3">
+        <f ca="1">NOW()</f>
+        <v>44519.838576620372</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C14" s="3">
         <v>44517.88040011574</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="3">
+        <v>44519.83730324074</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
@@ -967,29 +984,42 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C16" s="3">
         <v>44519.002479050927</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="3">
+        <f ca="1">NOW()</f>
+        <v>44519.838576620372</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C17" s="3">
-        <v>44519.807343749999</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
+        <v>44519.837528356482</v>
+      </c>
+      <c r="D17" s="3">
+        <v>44519.83730324074</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>

</xml_diff>